<commit_message>
Reorg folders and other mods
</commit_message>
<xml_diff>
--- a/sorel/01_bench_s3_ls/analysis/run notes.xlsx
+++ b/sorel/01_bench_s3_ls/analysis/run notes.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HERZOMJ\source\GitHub\big_data_demo\sorel\01. bench_s3_ls\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HERZOMJ\source\GitHub\big_data_demo\sorel\01_bench_s3_ls\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5CA91A-3321-4BF0-93FB-9D1120223C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE63D1-EE23-4257-90CE-73EE8B24250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C86255B7-07AE-4159-A1DE-F8879CE0F203}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{C86255B7-07AE-4159-A1DE-F8879CE0F203}"/>
   </bookViews>
   <sheets>
     <sheet name="List keys" sheetId="1" r:id="rId1"/>
     <sheet name="Copy files" sheetId="3" r:id="rId2"/>
     <sheet name="Requirements" sheetId="4" r:id="rId3"/>
+    <sheet name="Tieouts" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t xml:space="preserve">Start:  </t>
   </si>
@@ -162,6 +163,33 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>Prefix "0"</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Target (Athena query)</t>
+  </si>
+  <si>
+    <t>All objects</t>
+  </si>
+  <si>
+    <t>Meta table</t>
+  </si>
+  <si>
+    <t>Grep meta.csv</t>
+  </si>
+  <si>
+    <t>Parquet files</t>
+  </si>
+  <si>
+    <t>Binaries from s3 ls of source</t>
+  </si>
+  <si>
+    <t>Parquet query</t>
   </si>
 </sst>
 </file>
@@ -453,8 +481,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{46365901-7C69-40B0-AB8B-6EEFD7B856E7}" name="Table4" displayName="Table4" ref="A4:F7" totalsRowShown="0">
-  <autoFilter ref="A4:F7" xr:uid="{46365901-7C69-40B0-AB8B-6EEFD7B856E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{46365901-7C69-40B0-AB8B-6EEFD7B856E7}" name="Table4" displayName="Table4" ref="A4:F8" totalsRowShown="0">
+  <autoFilter ref="A4:F8" xr:uid="{46365901-7C69-40B0-AB8B-6EEFD7B856E7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A4245A19-B11D-4B9B-9800-AA9A2CF15EDC}" name="Time Required (Hrs)"/>
     <tableColumn id="2" xr3:uid="{8D8A9450-4CB7-4987-87A1-753AC4C8914F}" name="Files/Sec" dataDxfId="3">
@@ -778,21 +806,21 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -818,7 +846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45002</v>
       </c>
@@ -846,7 +874,7 @@
         <v>1233.4473472435425</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45002</v>
       </c>
@@ -874,7 +902,7 @@
         <v>1656.1264818903298</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45002</v>
       </c>
@@ -916,26 +944,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA2B0AC-F327-404A-B537-1167C600A620}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -979,7 +1009,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45002</v>
       </c>
@@ -1027,7 +1057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45002</v>
       </c>
@@ -1075,7 +1105,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45001</v>
       </c>
@@ -1121,7 +1151,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M5" s="5">
         <v>618932</v>
       </c>
@@ -1136,7 +1166,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M6" s="5">
         <v>13000000</v>
       </c>
@@ -1160,20 +1190,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2CF93B-46C4-4E6B-B55C-4199235AF246}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1181,7 +1213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>13000000</v>
       </c>
@@ -1189,7 +1221,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1209,7 +1241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1233,7 +1265,7 @@
         <v>222.22222222222223</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1257,7 +1289,7 @@
         <v>111.11111111111111</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1279,6 +1311,30 @@
       <c r="F7" s="9">
         <f>Table4[[#This Row],[MB/Sec]]/Table4[[#This Row],['# Workers]]</f>
         <v>11.111111111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9" cm="1">
+        <f t="array" ref="B8">Table3['# Files]/Table4[[#This Row],[Time Required (Hrs)]]/3600</f>
+        <v>361.11111111111109</v>
+      </c>
+      <c r="C8" s="5" cm="1">
+        <f t="array" ref="C8">Table3[Data to transfer (MB)]/Table4[[#This Row],[Time Required (Hrs)]]/3600</f>
+        <v>222.22222222222223</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8" s="9">
+        <f>Table4[[#This Row],[Files/Sec]]/Table4[[#This Row],['# Workers]]</f>
+        <v>22.569444444444443</v>
+      </c>
+      <c r="F8" s="9">
+        <f>Table4[[#This Row],[MB/Sec]]/Table4[[#This Row],['# Workers]]</f>
+        <v>13.888888888888889</v>
       </c>
     </row>
   </sheetData>
@@ -1288,4 +1344,82 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA42797-8E56-4D1C-B2D4-9722588A150D}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5">
+        <v>618932</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="5">
+        <v>19724998</v>
+      </c>
+      <c r="I3" s="5">
+        <v>378274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="5">
+        <v>618932</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5">
+        <v>9919065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1271809</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="5">
+        <v>9919065</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final code for v1.0
</commit_message>
<xml_diff>
--- a/sorel/01_bench_s3_ls/analysis/run notes.xlsx
+++ b/sorel/01_bench_s3_ls/analysis/run notes.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HERZOMJ\source\GitHub\big_data_demo\sorel\01_bench_s3_ls\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D39880-9F3C-4867-B2A5-59EC20AE22C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C28962-AB4C-4B7C-9581-283521AEF098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C86255B7-07AE-4159-A1DE-F8879CE0F203}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{C86255B7-07AE-4159-A1DE-F8879CE0F203}"/>
   </bookViews>
   <sheets>
     <sheet name="List keys" sheetId="1" r:id="rId1"/>
     <sheet name="Copy files" sheetId="3" r:id="rId2"/>
     <sheet name="Requirements" sheetId="4" r:id="rId3"/>
     <sheet name="Tieouts" sheetId="5" r:id="rId4"/>
+    <sheet name="Benchmarks" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t xml:space="preserve">Start:  </t>
   </si>
@@ -208,6 +209,54 @@
   </si>
   <si>
     <t>transfer_sorel_binaries_no_spark.py</t>
+  </si>
+  <si>
+    <t>Key Listing</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Elapsed</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>Athena</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>times faster</t>
+  </si>
+  <si>
+    <t>Copy all keys beginning with 00</t>
+  </si>
+  <si>
+    <t>s3 cp parquet</t>
+  </si>
+  <si>
+    <t>s3 cp sorel source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14G   </t>
+  </si>
+  <si>
+    <t>Size copied</t>
+  </si>
+  <si>
+    <t>Throughput</t>
+  </si>
+  <si>
+    <t>MB per second</t>
+  </si>
+  <si>
+    <t>9.9G</t>
   </si>
 </sst>
 </file>
@@ -219,7 +268,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +277,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -256,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -271,6 +328,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1276,7 +1334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2CF93B-46C4-4E6B-B55C-4199235AF246}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1562,4 +1620,201 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C695DB-E0C8-4521-B6B4-49138DFCEC79}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45002.577974537038</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="6">
+        <v>45007.257523148146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45002.592152777775</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="6">
+        <v>45007.265381944446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <f>(B5-B4)*24*60</f>
+        <v>20.416666661622003</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6">
+        <f>(G5-G4)*24*60</f>
+        <v>11.316666671773419</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>14811</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <f>59.806/60</f>
+        <v>0.99676666666666658</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="5">
+        <f>14000000000/G6/60</f>
+        <v>20618556.69172661</v>
+      </c>
+      <c r="H9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <f>B6/B9</f>
+        <v>20.482894687779158</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="6">
+        <v>45007.267465277779</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="6">
+        <v>45007.273043981484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14">
+        <f>(G13-G12)*24*60</f>
+        <v>8.0333333357702941</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="5">
+        <f>9900000000/G14/60</f>
+        <v>20539419.080906171</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>